<commit_message>
Fixed VK event, club records had as 10000m but actually 10K. Ditching source code link.
</commit_message>
<xml_diff>
--- a/2021_CnC_records.xlsx
+++ b/2021_CnC_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8816684-1FD3-4F80-8679-3D50D675F9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8CBE6A-94AC-480C-B451-6A0EEDFC8E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{55F626DB-26DF-4F6A-9259-B6403442FA4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{55F626DB-26DF-4F6A-9259-B6403442FA4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4460" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="1095">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3319,6 +3319,12 @@
   </si>
   <si>
     <t>4:39.54</t>
+  </si>
+  <si>
+    <t>CW: this was a 10K road race not track 10000m</t>
+  </si>
+  <si>
+    <t>10K</t>
   </si>
 </sst>
 </file>
@@ -9446,8 +9452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D17D48-6A09-4E8D-9C29-A364728CDDFA}">
   <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10109,7 +10115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
@@ -10117,7 +10123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>509</v>
       </c>
@@ -10143,7 +10149,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
@@ -10166,7 +10172,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
@@ -10189,7 +10195,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -10212,7 +10218,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>8</v>
       </c>
@@ -10235,7 +10241,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>10</v>
       </c>
@@ -10258,7 +10264,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
@@ -10281,7 +10287,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>491</v>
       </c>
@@ -10295,7 +10301,7 @@
         <v>492</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>990</v>
+        <v>1094</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>1037</v>
@@ -10303,8 +10309,11 @@
       <c r="H42" s="1" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
@@ -10327,7 +10336,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>512</v>
       </c>
@@ -10350,7 +10359,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>57</v>
       </c>
@@ -10373,7 +10382,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>59</v>
       </c>
@@ -10387,7 +10396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>18</v>
       </c>
@@ -10401,7 +10410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>62</v>
       </c>
@@ -14195,8 +14204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B8E74-193C-4A62-9827-E7761224CD25}">
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Corrected 'Dianna' typo in old club records that gave spurious entry
</commit_message>
<xml_diff>
--- a/2021_CnC_records.xlsx
+++ b/2021_CnC_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D527D3B3-DF0D-421E-A839-956B69F888A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90D3025-FED1-458C-8B69-144478820449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{55F626DB-26DF-4F6A-9259-B6403442FA4D}"/>
+    <workbookView xWindow="3384" yWindow="1644" windowWidth="17412" windowHeight="10704" xr2:uid="{55F626DB-26DF-4F6A-9259-B6403442FA4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4484" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4484" uniqueCount="1122">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3403,6 +3403,9 @@
   </si>
   <si>
     <t>Skipping this because PenIM35 age-group specific, also listed there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diana Chalmers </t>
   </si>
 </sst>
 </file>
@@ -4197,8 +4200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A31CADB-781F-4F55-B093-B2ED4E03C3FD}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5141,7 +5144,7 @@
         <v>135</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>60</v>
+        <v>1121</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>1030</v>

</xml_diff>